<commit_message>
changed ndvi calculations to S2A SRF
</commit_message>
<xml_diff>
--- a/data/2019/Data AGB BGB Bourgneuf 2019.xlsx
+++ b/data/2019/Data AGB BGB Bourgneuf 2019.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REWRITE\Field_data\Bourgneuf_spectra_2018_2025_comparison\data\2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\REWRITE\Field_data\Bourgneuf_spectra_2018_2025_comparison\data\2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -74,9 +74,6 @@
     <t>zos_07</t>
   </si>
   <si>
-    <t>zos_088</t>
-  </si>
-  <si>
     <t>zos_09</t>
   </si>
   <si>
@@ -141,6 +138,9 @@
   </si>
   <si>
     <t>zos_30</t>
+  </si>
+  <si>
+    <t>zos_08</t>
   </si>
 </sst>
 </file>
@@ -473,7 +473,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,7 +629,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="B9" s="3">
         <v>28.722999999999999</v>
@@ -648,7 +648,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" s="3">
         <v>27.663</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" s="3">
         <v>9.2149999999999999</v>
@@ -686,7 +686,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="3">
         <v>24.109000000000002</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B13" s="3">
         <v>7.72</v>
@@ -724,7 +724,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B14" s="3">
         <v>24.219000000000001</v>
@@ -743,7 +743,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3">
         <v>26.809000000000001</v>
@@ -762,7 +762,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B16" s="3">
         <v>50.094000000000001</v>
@@ -781,7 +781,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B17" s="3">
         <v>127.14100000000001</v>
@@ -800,7 +800,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="3">
         <v>53.683999999999997</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B19" s="3">
         <v>110.816</v>
@@ -838,7 +838,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="3">
         <v>39.902999999999999</v>
@@ -857,7 +857,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B21" s="3">
         <v>54.718000000000004</v>
@@ -876,7 +876,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" s="3">
         <v>51.746000000000002</v>
@@ -895,7 +895,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" s="3">
         <v>54.777999999999999</v>
@@ -914,7 +914,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" s="3">
         <v>42.192999999999998</v>
@@ -933,7 +933,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" s="3">
         <v>48.58</v>
@@ -952,7 +952,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" s="3">
         <v>34.798000000000002</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" s="3">
         <v>45.445</v>
@@ -990,7 +990,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" s="3">
         <v>38.076000000000001</v>
@@ -1009,7 +1009,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B29" s="3">
         <v>33.024999999999999</v>
@@ -1026,7 +1026,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B30" s="3">
         <v>37.51</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B31" s="3">
         <v>32.848999999999997</v>

</xml_diff>